<commit_message>
kiz() and alg2() only take 'df' and 'tb'. rename 'check_eligibility'. kiz is only paid for kindergeld-kinder
Former-commit-id: 658d9ba8c5fa0a261968cc1cf04555e2c691f125
Former-commit-id: e931fea5e8efe3b112d57b799f3797a82f6e692e
</commit_message>
<xml_diff>
--- a/tests/test_tax_transfers/test_data/test_dfs_kiz.xlsx
+++ b/tests/test_tax_transfers/test_data/test_dfs_kiz.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>hid</t>
   </si>
@@ -137,6 +137,15 @@
   </si>
   <si>
     <t>pid</t>
+  </si>
+  <si>
+    <t>w_hours</t>
+  </si>
+  <si>
+    <t>m_wage</t>
+  </si>
+  <si>
+    <t>ineducation</t>
   </si>
 </sst>
 </file>
@@ -544,24 +553,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ42"/>
+  <dimension ref="A1:AT42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="25" max="25" width="8.85546875" customWidth="1"/>
-    <col min="27" max="27" width="11.28515625" customWidth="1"/>
-    <col min="29" max="29" width="12.5703125" customWidth="1"/>
-    <col min="30" max="30" width="14.7109375" customWidth="1"/>
-    <col min="31" max="31" width="14.7109375" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="16.140625" customWidth="1"/>
-    <col min="33" max="33" width="9.28515625" customWidth="1"/>
+    <col min="28" max="28" width="8.85546875" customWidth="1"/>
+    <col min="30" max="30" width="11.28515625" customWidth="1"/>
+    <col min="32" max="32" width="12.5703125" customWidth="1"/>
+    <col min="33" max="33" width="14.7109375" customWidth="1"/>
+    <col min="34" max="34" width="14.7109375" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="16.140625" customWidth="1"/>
+    <col min="36" max="36" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -593,102 +602,111 @@
         <v>9</v>
       </c>
       <c r="K1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="T1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="U1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="V1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="W1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="X1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="Y1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="Z1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="AA1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="AB1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="AC1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="13" t="s">
+      <c r="AD1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12" t="s">
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="AD1" s="12" t="s">
+      <c r="AG1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="23" t="s">
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="AG1" s="12" t="s">
+      <c r="AJ1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="AH1" s="12" t="s">
+      <c r="AK1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="AI1" s="12" t="s">
+      <c r="AL1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="AJ1" s="12" t="s">
+      <c r="AM1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="AK1" s="12" t="s">
+      <c r="AN1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="AL1" s="12" t="s">
+      <c r="AO1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="AM1" s="12" t="s">
+      <c r="AP1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="AN1" s="12" t="s">
+      <c r="AQ1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="AO1" s="12" t="s">
+      <c r="AR1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="AP1" s="12" t="s">
+      <c r="AS1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="AQ1" s="12" t="s">
+      <c r="AT1" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>B2</f>
         <v>1</v>
@@ -721,120 +739,130 @@
         <v>30</v>
       </c>
       <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <f>IF(J2&gt;18,2000,0)</f>
+        <v>2000</v>
+      </c>
+      <c r="M2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2">
         <v>700</v>
       </c>
-      <c r="L2">
+      <c r="O2">
         <v>100</v>
       </c>
-      <c r="M2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <f t="shared" ref="O2:O13" si="0">G2-P2</f>
+      <c r="P2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <f t="shared" ref="R2:R13" si="0">G2-S2</f>
         <v>2</v>
       </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
         <v>1200</v>
       </c>
-      <c r="R2" s="2">
+      <c r="U2" s="2">
         <v>644</v>
       </c>
-      <c r="S2" s="2">
+      <c r="V2" s="2">
         <v>350</v>
       </c>
-      <c r="T2" s="3">
+      <c r="W2" s="3">
         <v>1765</v>
       </c>
-      <c r="U2" s="3">
+      <c r="X2" s="3">
         <v>1300</v>
       </c>
-      <c r="V2">
-        <f>P2*190</f>
+      <c r="Y2">
+        <f>S2*190</f>
         <v>190</v>
       </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
         <v>2016</v>
       </c>
-      <c r="Y2" s="1">
-        <f>IF(OR($AP2=TRUE,$AQ2=TRUE),$AJ2,0)</f>
+      <c r="AB2" s="1">
+        <f>IF(OR($AS2=TRUE,$AT2=TRUE),$AM2,0)</f>
         <v>140</v>
       </c>
-      <c r="Z2" s="1">
-        <f>IF(AND($AO2=FALSE,$AP2=FALSE,$AQ2=FALSE),$AK2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AA2" s="1">
-        <f>IF(OR($AO2=TRUE,$AQ2=TRUE),$S2,0)</f>
+      <c r="AC2" s="1">
+        <f>IF(AND($AR2=FALSE,$AS2=FALSE,$AT2=FALSE),$AN2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD2" s="1">
+        <f>IF(OR($AR2=TRUE,$AT2=TRUE),$V2,0)</f>
         <v>350</v>
       </c>
-      <c r="AC2">
+      <c r="AF2">
         <f>2*364</f>
         <v>728</v>
       </c>
-      <c r="AD2" s="8">
-        <f>0.8316*(K2+L2)</f>
+      <c r="AG2" s="8">
+        <f>0.8316*(N2+O2)</f>
         <v>665.28</v>
       </c>
-      <c r="AE2" s="8"/>
-      <c r="AF2" s="24">
-        <f>AC2+AD2</f>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="24">
+        <f>AF2+AG2</f>
         <v>1393.28</v>
       </c>
-      <c r="AG2" s="10">
-        <f>AF2+170*P2</f>
+      <c r="AJ2" s="10">
+        <f>AI2+170*S2</f>
         <v>1563.28</v>
       </c>
-      <c r="AH2" t="b">
-        <f>AND((Q2&gt;900),(R2&lt;=AG2))</f>
-        <v>1</v>
-      </c>
-      <c r="AI2" s="8">
-        <f>ROUND(MAX(R2-AF2,0)/10,0)*5</f>
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="8">
-        <f t="shared" ref="AJ2:AJ13" si="1">AH2*140*P2-AI2</f>
+      <c r="AK2" t="b">
+        <f>AND((T2&gt;900),(U2&lt;=AJ2))</f>
+        <v>1</v>
+      </c>
+      <c r="AL2" s="8">
+        <f>ROUND(MAX(U2-AI2,0)/10,0)*5</f>
+        <v>0</v>
+      </c>
+      <c r="AM2" s="8">
+        <f t="shared" ref="AM2:AM13" si="1">AK2*140*S2-AL2</f>
         <v>140</v>
       </c>
-      <c r="AK2" s="28">
-        <f>MAX(T2-U2,0)</f>
+      <c r="AN2" s="28">
+        <f>MAX(W2-X2,0)</f>
         <v>465</v>
       </c>
-      <c r="AL2" s="28">
-        <f>MAX(T2-U2-S2,0)</f>
+      <c r="AO2" s="28">
+        <f>MAX(W2-X2-V2,0)</f>
         <v>115</v>
       </c>
-      <c r="AM2" s="28">
-        <f>MAX(T2-U2-AJ2,0)</f>
+      <c r="AP2" s="28">
+        <f>MAX(W2-X2-AM2,0)</f>
         <v>325</v>
       </c>
-      <c r="AN2" s="28">
-        <f>MAX(T2-U2-S2-AJ2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AO2" t="b">
-        <f>AND(AL2=0,AK2&gt;0)</f>
-        <v>0</v>
-      </c>
-      <c r="AP2" t="b">
-        <f>AND(AM2=0,AK2&gt;0)</f>
-        <v>0</v>
-      </c>
-      <c r="AQ2" t="b">
-        <f>AND(AN2=0,AK2&gt;0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ2" s="28">
+        <f>MAX(W2-X2-V2-AM2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AR2" t="b">
+        <f>AND(AO2=0,AN2&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="AS2" t="b">
+        <f>AND(AP2=0,AN2&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="AT2" t="b">
+        <f>AND(AQ2=0,AN2&gt;0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -866,120 +894,130 @@
         <v>30</v>
       </c>
       <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L18" si="2">IF(J3&gt;18,2000,0)</f>
+        <v>2000</v>
+      </c>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3">
         <v>700</v>
       </c>
-      <c r="L3">
+      <c r="O3">
         <v>100</v>
       </c>
-      <c r="M3" t="b">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
+      <c r="P3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3">
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
         <v>1200</v>
       </c>
-      <c r="R3" s="3">
+      <c r="U3" s="3">
         <v>644</v>
       </c>
-      <c r="S3" s="3">
+      <c r="V3" s="3">
         <v>350</v>
       </c>
-      <c r="T3" s="3">
+      <c r="W3" s="3">
         <v>1765</v>
       </c>
-      <c r="U3" s="3">
+      <c r="X3" s="3">
         <v>1300</v>
       </c>
-      <c r="V3">
-        <f>P3*190</f>
+      <c r="Y3">
+        <f>S3*190</f>
         <v>190</v>
       </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3">
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
         <v>2016</v>
       </c>
-      <c r="Y3" s="11">
-        <f t="shared" ref="Y3:Y16" si="2">IF(OR($AP3=TRUE,$AQ3=TRUE),$AJ3,0)</f>
+      <c r="AB3" s="11">
+        <f t="shared" ref="AB3:AB16" si="3">IF(OR($AS3=TRUE,$AT3=TRUE),$AM3,0)</f>
         <v>140</v>
       </c>
-      <c r="Z3" s="1">
-        <f t="shared" ref="Z3:Z18" si="3">IF(AND($AO3=FALSE,$AP3=FALSE,$AQ3=FALSE),$AK3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AA3" s="1">
-        <f t="shared" ref="AA3:AA18" si="4">IF(OR($AO3=TRUE,$AQ3=TRUE),$S3,0)</f>
+      <c r="AC3" s="1">
+        <f t="shared" ref="AC3:AC18" si="4">IF(AND($AR3=FALSE,$AS3=FALSE,$AT3=FALSE),$AN3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD3" s="1">
+        <f t="shared" ref="AD3:AD18" si="5">IF(OR($AR3=TRUE,$AT3=TRUE),$V3,0)</f>
         <v>350</v>
       </c>
-      <c r="AC3">
-        <f t="shared" ref="AC3:AC4" si="5">2*364</f>
+      <c r="AF3">
+        <f t="shared" ref="AF3:AF4" si="6">2*364</f>
         <v>728</v>
       </c>
-      <c r="AD3" s="8">
-        <f t="shared" ref="AD3:AD4" si="6">0.8316*(K3+L3)</f>
+      <c r="AG3" s="8">
+        <f t="shared" ref="AG3:AG4" si="7">0.8316*(N3+O3)</f>
         <v>665.28</v>
       </c>
-      <c r="AE3" s="8"/>
-      <c r="AF3" s="24">
-        <f t="shared" ref="AF3:AF16" si="7">AC3+AD3</f>
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="24">
+        <f t="shared" ref="AI3:AI16" si="8">AF3+AG3</f>
         <v>1393.28</v>
       </c>
-      <c r="AG3" s="10">
-        <f t="shared" ref="AG3:AG4" si="8">AF3+170*P3</f>
+      <c r="AJ3" s="10">
+        <f t="shared" ref="AJ3:AJ4" si="9">AI3+170*S3</f>
         <v>1563.28</v>
       </c>
-      <c r="AH3" t="b">
-        <f t="shared" ref="AH3:AH13" si="9">AND((Q3&gt;900),(R3&lt;=AG3))</f>
-        <v>1</v>
-      </c>
-      <c r="AI3">
-        <f t="shared" ref="AI3:AI16" si="10">ROUND(MAX(R3-AF3,0)/10,0)*5</f>
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="8">
+      <c r="AK3" t="b">
+        <f t="shared" ref="AK3:AK13" si="10">AND((T3&gt;900),(U3&lt;=AJ3))</f>
+        <v>1</v>
+      </c>
+      <c r="AL3">
+        <f t="shared" ref="AL3:AL16" si="11">ROUND(MAX(U3-AI3,0)/10,0)*5</f>
+        <v>0</v>
+      </c>
+      <c r="AM3" s="8">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="AK3" s="28">
-        <f t="shared" ref="AK3:AK16" si="11">MAX(T3-U3,0)</f>
+      <c r="AN3" s="28">
+        <f t="shared" ref="AN3:AN16" si="12">MAX(W3-X3,0)</f>
         <v>465</v>
       </c>
-      <c r="AL3" s="28">
-        <f t="shared" ref="AL3:AL16" si="12">MAX(T3-U3-S3,0)</f>
+      <c r="AO3" s="28">
+        <f t="shared" ref="AO3:AO16" si="13">MAX(W3-X3-V3,0)</f>
         <v>115</v>
       </c>
-      <c r="AM3" s="28">
-        <f t="shared" ref="AM3:AM16" si="13">MAX(T3-U3-AJ3,0)</f>
+      <c r="AP3" s="28">
+        <f t="shared" ref="AP3:AP16" si="14">MAX(W3-X3-AM3,0)</f>
         <v>325</v>
       </c>
-      <c r="AN3" s="28">
-        <f t="shared" ref="AN3:AN16" si="14">MAX(T3-U3-S3-AJ3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AO3" t="b">
-        <f t="shared" ref="AO3:AO16" si="15">AND(AL3=0,AK3&gt;0)</f>
-        <v>0</v>
-      </c>
-      <c r="AP3" t="b">
-        <f t="shared" ref="AP3:AP16" si="16">AND(AM3=0,AK3&gt;0)</f>
-        <v>0</v>
-      </c>
-      <c r="AQ3" t="b">
-        <f t="shared" ref="AQ3:AQ16" si="17">AND(AN3=0,AK3&gt;0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ3" s="28">
+        <f t="shared" ref="AQ3:AQ16" si="15">MAX(W3-X3-V3-AM3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AR3" t="b">
+        <f t="shared" ref="AR3:AR16" si="16">AND(AO3=0,AN3&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="AS3" t="b">
+        <f t="shared" ref="AS3:AS16" si="17">AND(AP3=0,AN3&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="AT3" t="b">
+        <f t="shared" ref="AT3:AT16" si="18">AND(AQ3=0,AN3&gt;0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1011,120 +1049,130 @@
         <v>2</v>
       </c>
       <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4">
         <v>700</v>
       </c>
-      <c r="L4">
+      <c r="O4">
         <v>100</v>
       </c>
-      <c r="M4" t="b">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
+      <c r="P4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4">
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
         <v>1200</v>
       </c>
-      <c r="R4">
+      <c r="U4">
         <v>644</v>
       </c>
-      <c r="S4">
+      <c r="V4">
         <v>350</v>
       </c>
-      <c r="T4">
+      <c r="W4">
         <v>1765</v>
       </c>
-      <c r="U4">
+      <c r="X4">
         <v>1300</v>
       </c>
-      <c r="V4">
-        <f>P4*190</f>
+      <c r="Y4">
+        <f>S4*190</f>
         <v>190</v>
       </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
         <v>2016</v>
       </c>
-      <c r="Y4" s="11">
-        <f t="shared" si="2"/>
+      <c r="AB4" s="11">
+        <f t="shared" si="3"/>
         <v>140</v>
       </c>
-      <c r="Z4" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AA4" s="1">
+      <c r="AC4" s="1">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AD4" s="1">
+        <f t="shared" si="5"/>
         <v>350</v>
       </c>
-      <c r="AC4">
-        <f t="shared" si="5"/>
+      <c r="AF4">
+        <f t="shared" si="6"/>
         <v>728</v>
       </c>
-      <c r="AD4" s="8">
-        <f t="shared" si="6"/>
+      <c r="AG4" s="8">
+        <f t="shared" si="7"/>
         <v>665.28</v>
       </c>
-      <c r="AE4" s="8"/>
-      <c r="AF4" s="24">
-        <f t="shared" si="7"/>
+      <c r="AH4" s="8"/>
+      <c r="AI4" s="24">
+        <f t="shared" si="8"/>
         <v>1393.28</v>
       </c>
-      <c r="AG4" s="10">
-        <f t="shared" si="8"/>
+      <c r="AJ4" s="10">
+        <f t="shared" si="9"/>
         <v>1563.28</v>
       </c>
-      <c r="AH4" t="b">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AI4">
+      <c r="AK4" t="b">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AJ4" s="8">
+        <v>1</v>
+      </c>
+      <c r="AL4">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AM4" s="8">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="AK4" s="28">
-        <f t="shared" si="11"/>
+      <c r="AN4" s="28">
+        <f t="shared" si="12"/>
         <v>465</v>
       </c>
-      <c r="AL4" s="28">
-        <f t="shared" si="12"/>
+      <c r="AO4" s="28">
+        <f t="shared" si="13"/>
         <v>115</v>
       </c>
-      <c r="AM4" s="28">
-        <f t="shared" si="13"/>
+      <c r="AP4" s="28">
+        <f t="shared" si="14"/>
         <v>325</v>
       </c>
-      <c r="AN4" s="28">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AO4" t="b">
+      <c r="AQ4" s="28">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AP4" t="b">
+      <c r="AR4" t="b">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AQ4" t="b">
+      <c r="AS4" t="b">
         <f t="shared" si="17"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="AT4" t="b">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1156,111 +1204,121 @@
         <v>40</v>
       </c>
       <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>2000</v>
+      </c>
+      <c r="M5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
         <v>400</v>
       </c>
-      <c r="L5" s="2">
+      <c r="O5" s="2">
         <v>80</v>
       </c>
-      <c r="M5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2">
-        <v>0</v>
-      </c>
-      <c r="O5" s="2">
+      <c r="P5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="P5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2">
+      <c r="S5" s="2">
+        <v>0</v>
+      </c>
+      <c r="T5" s="2">
         <v>800</v>
       </c>
-      <c r="R5" s="2">
+      <c r="U5" s="2">
         <v>512</v>
       </c>
-      <c r="S5" s="2">
+      <c r="V5" s="2">
         <v>400</v>
       </c>
-      <c r="T5" s="2">
+      <c r="W5" s="2">
         <v>1170</v>
       </c>
-      <c r="U5" s="2">
+      <c r="X5" s="2">
         <v>700</v>
       </c>
-      <c r="V5" s="2">
-        <v>0</v>
-      </c>
-      <c r="W5" s="2">
-        <v>0</v>
-      </c>
-      <c r="X5" s="2">
+      <c r="Y5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="2">
         <v>2013</v>
       </c>
-      <c r="Y5" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z5" s="1">
+      <c r="AB5" s="20">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AC5" s="1">
+        <f t="shared" si="4"/>
         <v>470</v>
       </c>
-      <c r="AA5" s="18">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB5" s="2"/>
-      <c r="AC5" s="2">
+      <c r="AD5" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2">
         <f>2*345</f>
         <v>690</v>
       </c>
-      <c r="AD5" s="9"/>
-      <c r="AE5" s="8"/>
-      <c r="AF5" s="25">
-        <f t="shared" si="7"/>
+      <c r="AG5" s="9"/>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="25">
+        <f t="shared" si="8"/>
         <v>690</v>
       </c>
-      <c r="AG5" s="14"/>
-      <c r="AH5" s="2"/>
-      <c r="AI5" s="2">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AJ5" s="9">
+      <c r="AJ5" s="14"/>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AM5" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AK5" s="29">
-        <f t="shared" si="11"/>
+      <c r="AN5" s="29">
+        <f t="shared" si="12"/>
         <v>470</v>
       </c>
-      <c r="AL5" s="29">
-        <f t="shared" si="12"/>
+      <c r="AO5" s="29">
+        <f t="shared" si="13"/>
         <v>70</v>
       </c>
-      <c r="AM5" s="29">
-        <f t="shared" si="13"/>
+      <c r="AP5" s="29">
+        <f t="shared" si="14"/>
         <v>470</v>
       </c>
-      <c r="AN5" s="28">
-        <f t="shared" si="14"/>
+      <c r="AQ5" s="28">
+        <f t="shared" si="15"/>
         <v>70</v>
       </c>
-      <c r="AO5" t="b">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AP5" t="b">
+      <c r="AR5" t="b">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AQ5" t="b">
+      <c r="AS5" t="b">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT5" t="b">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1291,111 +1349,121 @@
       <c r="J6" s="3">
         <v>40</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>2000</v>
+      </c>
+      <c r="M6" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" s="5">
         <v>400</v>
       </c>
-      <c r="L6" s="5">
+      <c r="O6" s="5">
         <v>80</v>
       </c>
-      <c r="M6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N6" s="6">
-        <v>0</v>
-      </c>
-      <c r="O6" s="6">
+      <c r="P6" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>0</v>
+      </c>
+      <c r="R6" s="6">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="P6" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="6">
+      <c r="S6" s="6">
+        <v>0</v>
+      </c>
+      <c r="T6" s="6">
         <v>800</v>
       </c>
-      <c r="R6" s="6">
+      <c r="U6" s="6">
         <v>512</v>
       </c>
-      <c r="S6" s="6">
+      <c r="V6" s="6">
         <v>400</v>
       </c>
-      <c r="T6" s="6">
+      <c r="W6" s="6">
         <v>1170</v>
       </c>
-      <c r="U6" s="6">
+      <c r="X6" s="6">
         <v>700</v>
       </c>
-      <c r="V6" s="3">
-        <v>0</v>
-      </c>
-      <c r="W6" s="3">
-        <v>0</v>
-      </c>
-      <c r="X6" s="3">
+      <c r="Y6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="3">
         <v>2013</v>
       </c>
-      <c r="Y6" s="21">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z6" s="1">
+      <c r="AB6" s="21">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AC6" s="1">
+        <f t="shared" si="4"/>
         <v>470</v>
       </c>
-      <c r="AA6" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AC6" s="6">
+      <c r="AD6" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AF6" s="6">
         <f>2*345</f>
         <v>690</v>
       </c>
-      <c r="AD6" s="8"/>
-      <c r="AE6" s="8"/>
-      <c r="AF6" s="26">
-        <f t="shared" si="7"/>
+      <c r="AG6" s="8"/>
+      <c r="AH6" s="8"/>
+      <c r="AI6" s="26">
+        <f t="shared" si="8"/>
         <v>690</v>
       </c>
-      <c r="AG6" s="16"/>
-      <c r="AH6" s="5"/>
-      <c r="AI6" s="3">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AJ6" s="17">
+      <c r="AJ6" s="16"/>
+      <c r="AK6" s="5"/>
+      <c r="AL6" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AM6" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AK6" s="30">
-        <f t="shared" si="11"/>
+      <c r="AN6" s="30">
+        <f t="shared" si="12"/>
         <v>470</v>
       </c>
-      <c r="AL6" s="30">
-        <f t="shared" si="12"/>
+      <c r="AO6" s="30">
+        <f t="shared" si="13"/>
         <v>70</v>
       </c>
-      <c r="AM6" s="30">
-        <f t="shared" si="13"/>
+      <c r="AP6" s="30">
+        <f t="shared" si="14"/>
         <v>470</v>
       </c>
-      <c r="AN6" s="28">
-        <f t="shared" si="14"/>
+      <c r="AQ6" s="28">
+        <f t="shared" si="15"/>
         <v>70</v>
       </c>
-      <c r="AO6" t="b">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AP6" t="b">
+      <c r="AR6" t="b">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AQ6" t="b">
+      <c r="AS6" t="b">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT6" t="b">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -1427,120 +1495,130 @@
         <v>28</v>
       </c>
       <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>2000</v>
+      </c>
+      <c r="M7" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
         <v>400</v>
       </c>
-      <c r="L7" s="2">
+      <c r="O7" s="2">
         <v>80</v>
       </c>
-      <c r="M7" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="N7" s="2">
+      <c r="P7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="2">
         <v>0.36</v>
       </c>
-      <c r="O7" s="2">
+      <c r="R7" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="P7" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="2">
+      <c r="S7" s="2">
+        <v>1</v>
+      </c>
+      <c r="T7" s="2">
         <v>1000</v>
       </c>
-      <c r="R7" s="2">
+      <c r="U7" s="2">
         <v>719</v>
       </c>
-      <c r="S7" s="2">
+      <c r="V7" s="2">
         <v>500</v>
       </c>
-      <c r="T7" s="2">
+      <c r="W7" s="2">
         <v>1183.6399999999999</v>
       </c>
-      <c r="U7" s="2">
+      <c r="X7" s="2">
         <v>555</v>
       </c>
-      <c r="V7" s="2">
+      <c r="Y7" s="2">
         <v>164</v>
       </c>
-      <c r="W7" s="2">
-        <v>0</v>
-      </c>
-      <c r="X7" s="2">
+      <c r="Z7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="2">
         <v>2009</v>
       </c>
-      <c r="Y7" s="20">
-        <f t="shared" si="2"/>
+      <c r="AB7" s="20">
+        <f t="shared" si="3"/>
         <v>140</v>
       </c>
-      <c r="Z7" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AA7" s="18">
+      <c r="AC7" s="1">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AD7" s="18">
+        <f t="shared" si="5"/>
         <v>500</v>
       </c>
-      <c r="AB7" s="2"/>
-      <c r="AC7" s="4">
-        <f>359*(1+N7)</f>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="4">
+        <f>359*(1+Q7)</f>
         <v>488.23999999999995</v>
       </c>
-      <c r="AD7" s="9">
-        <f>0.759*(K7+L7)</f>
+      <c r="AG7" s="9">
+        <f>0.759*(N7+O7)</f>
         <v>364.32</v>
       </c>
-      <c r="AE7" s="8"/>
-      <c r="AF7" s="25">
-        <f t="shared" si="7"/>
+      <c r="AH7" s="8"/>
+      <c r="AI7" s="25">
+        <f t="shared" si="8"/>
         <v>852.56</v>
       </c>
-      <c r="AG7" s="10">
-        <f>AF7+140*P7</f>
+      <c r="AJ7" s="10">
+        <f>AI7+140*S7</f>
         <v>992.56</v>
       </c>
-      <c r="AH7" t="b">
-        <f>AND((Q7&gt;600),(R7&lt;=AG7))</f>
-        <v>1</v>
-      </c>
-      <c r="AI7">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AJ7" s="9">
+      <c r="AK7" t="b">
+        <f>AND((T7&gt;600),(U7&lt;=AJ7))</f>
+        <v>1</v>
+      </c>
+      <c r="AL7">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AM7" s="9">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="AK7" s="29">
-        <f t="shared" si="11"/>
+      <c r="AN7" s="29">
+        <f t="shared" si="12"/>
         <v>628.63999999999987</v>
       </c>
-      <c r="AL7" s="29">
-        <f t="shared" si="12"/>
+      <c r="AO7" s="29">
+        <f t="shared" si="13"/>
         <v>128.63999999999987</v>
       </c>
-      <c r="AM7" s="29">
-        <f t="shared" si="13"/>
+      <c r="AP7" s="29">
+        <f t="shared" si="14"/>
         <v>488.63999999999987</v>
       </c>
-      <c r="AN7" s="28">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AO7" t="b">
+      <c r="AQ7" s="28">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AP7" t="b">
+      <c r="AR7" t="b">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AQ7" t="b">
+      <c r="AS7" t="b">
         <f t="shared" si="17"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="AT7" t="b">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1572,119 +1650,129 @@
         <v>1</v>
       </c>
       <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M8" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" s="3">
         <v>400</v>
       </c>
-      <c r="L8" s="3">
+      <c r="O8" s="3">
         <v>80</v>
       </c>
-      <c r="M8" t="b">
-        <v>1</v>
-      </c>
-      <c r="N8" s="3">
+      <c r="P8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="3">
         <v>0.36</v>
       </c>
-      <c r="O8">
+      <c r="R8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="P8" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="3">
+      <c r="S8" s="3">
+        <v>1</v>
+      </c>
+      <c r="T8" s="3">
         <v>1000</v>
       </c>
-      <c r="R8" s="3">
+      <c r="U8" s="3">
         <v>719</v>
       </c>
-      <c r="S8" s="3">
+      <c r="V8" s="3">
         <v>500</v>
       </c>
-      <c r="T8" s="3">
+      <c r="W8" s="3">
         <v>1183.6399999999999</v>
       </c>
-      <c r="U8" s="2">
+      <c r="X8" s="2">
         <v>555</v>
       </c>
-      <c r="V8" s="3">
+      <c r="Y8" s="3">
         <v>164</v>
       </c>
-      <c r="W8" s="3">
-        <v>0</v>
-      </c>
-      <c r="X8" s="3">
+      <c r="Z8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="3">
         <v>2009</v>
       </c>
-      <c r="Y8" s="21">
-        <f t="shared" si="2"/>
+      <c r="AB8" s="21">
+        <f t="shared" si="3"/>
         <v>140</v>
       </c>
-      <c r="Z8" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AA8" s="19">
+      <c r="AC8" s="1">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AD8" s="19">
+        <f t="shared" si="5"/>
         <v>500</v>
       </c>
-      <c r="AC8" s="4">
-        <f>359*(1+N8)</f>
+      <c r="AF8" s="4">
+        <f>359*(1+Q8)</f>
         <v>488.23999999999995</v>
       </c>
-      <c r="AD8" s="8">
-        <f>0.759*(K8+L8)</f>
+      <c r="AG8" s="8">
+        <f>0.759*(N8+O8)</f>
         <v>364.32</v>
       </c>
-      <c r="AE8" s="8"/>
-      <c r="AF8" s="27">
-        <f t="shared" si="7"/>
+      <c r="AH8" s="8"/>
+      <c r="AI8" s="27">
+        <f t="shared" si="8"/>
         <v>852.56</v>
       </c>
-      <c r="AG8" s="10">
-        <f>AF8+140*P8</f>
+      <c r="AJ8" s="10">
+        <f>AI8+140*S8</f>
         <v>992.56</v>
       </c>
-      <c r="AH8" s="3" t="b">
-        <f>AND((Q8&gt;600),(R8&lt;=AG8))</f>
-        <v>1</v>
-      </c>
-      <c r="AI8" s="3">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AJ8" s="8">
+      <c r="AK8" s="3" t="b">
+        <f>AND((T8&gt;600),(U8&lt;=AJ8))</f>
+        <v>1</v>
+      </c>
+      <c r="AL8" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AM8" s="8">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="AK8" s="31">
-        <f t="shared" si="11"/>
+      <c r="AN8" s="31">
+        <f t="shared" si="12"/>
         <v>628.63999999999987</v>
       </c>
-      <c r="AL8" s="31">
-        <f t="shared" si="12"/>
+      <c r="AO8" s="31">
+        <f t="shared" si="13"/>
         <v>128.63999999999987</v>
       </c>
-      <c r="AM8" s="31">
-        <f t="shared" si="13"/>
+      <c r="AP8" s="31">
+        <f t="shared" si="14"/>
         <v>488.63999999999987</v>
       </c>
-      <c r="AN8" s="28">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AO8" t="b">
+      <c r="AQ8" s="28">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AP8" t="b">
+      <c r="AR8" t="b">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AQ8" t="b">
+      <c r="AS8" t="b">
         <f t="shared" si="17"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="AT8" t="b">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>4</v>
       </c>
@@ -1716,121 +1804,131 @@
         <v>33</v>
       </c>
       <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>2000</v>
+      </c>
+      <c r="M9" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2">
         <v>850</v>
       </c>
-      <c r="L9" s="2">
+      <c r="O9" s="2">
         <v>120</v>
       </c>
-      <c r="M9" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N9" s="2">
-        <v>0</v>
-      </c>
-      <c r="O9" s="2">
+      <c r="P9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>0</v>
+      </c>
+      <c r="R9" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="P9" s="2">
+      <c r="S9" s="2">
         <v>3</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="T9" s="2">
         <v>2000</v>
       </c>
-      <c r="R9" s="2">
+      <c r="U9" s="2">
         <v>1500</v>
       </c>
-      <c r="S9" s="2">
+      <c r="V9" s="2">
         <v>650</v>
       </c>
-      <c r="T9" s="2">
+      <c r="W9" s="2">
         <v>2281</v>
       </c>
-      <c r="U9" s="2">
+      <c r="X9" s="2">
         <v>462</v>
       </c>
-      <c r="V9" s="2">
+      <c r="Y9" s="2">
         <f>3*154</f>
         <v>462</v>
       </c>
-      <c r="W9" s="2">
-        <v>0</v>
-      </c>
-      <c r="X9" s="2">
+      <c r="Z9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="2">
         <v>2006</v>
       </c>
-      <c r="Y9" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z9" s="1">
+      <c r="AB9" s="20">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AC9" s="1">
+        <f t="shared" si="4"/>
         <v>1819</v>
       </c>
-      <c r="AA9" s="18">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB9" s="2"/>
-      <c r="AC9" s="2">
+      <c r="AD9" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2">
         <f>345*0.9*2</f>
         <v>621</v>
       </c>
-      <c r="AD9" s="9">
-        <f>0.6212*(K9+L9)</f>
+      <c r="AG9" s="9">
+        <f>0.6212*(N9+O9)</f>
         <v>602.56399999999996</v>
       </c>
-      <c r="AE9" s="9"/>
-      <c r="AF9" s="25">
-        <f t="shared" si="7"/>
+      <c r="AH9" s="9"/>
+      <c r="AI9" s="25">
+        <f t="shared" si="8"/>
         <v>1223.5639999999999</v>
       </c>
-      <c r="AG9" s="14">
-        <f t="shared" ref="AG9:AG13" si="18">AF9+140*P9</f>
+      <c r="AJ9" s="14">
+        <f t="shared" ref="AJ9:AJ13" si="19">AI9+140*S9</f>
         <v>1643.5639999999999</v>
       </c>
-      <c r="AH9" s="2" t="b">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AI9" s="2">
+      <c r="AK9" s="2" t="b">
         <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AL9" s="2">
+        <f t="shared" si="11"/>
         <v>140</v>
       </c>
-      <c r="AJ9" s="9">
+      <c r="AM9" s="9">
         <f t="shared" si="1"/>
         <v>280</v>
       </c>
-      <c r="AK9" s="32">
-        <f t="shared" si="11"/>
+      <c r="AN9" s="32">
+        <f t="shared" si="12"/>
         <v>1819</v>
       </c>
-      <c r="AL9" s="29">
-        <f t="shared" si="12"/>
+      <c r="AO9" s="29">
+        <f t="shared" si="13"/>
         <v>1169</v>
       </c>
-      <c r="AM9" s="32">
-        <f t="shared" si="13"/>
+      <c r="AP9" s="32">
+        <f t="shared" si="14"/>
         <v>1539</v>
       </c>
-      <c r="AN9" s="28">
-        <f t="shared" si="14"/>
+      <c r="AQ9" s="28">
+        <f t="shared" si="15"/>
         <v>889</v>
       </c>
-      <c r="AO9" t="b">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AP9" t="b">
+      <c r="AR9" t="b">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AQ9" t="b">
+      <c r="AS9" t="b">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT9" t="b">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1861,121 +1959,131 @@
       <c r="J10" s="3">
         <v>30</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>2000</v>
+      </c>
+      <c r="M10" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" s="4">
         <v>850</v>
       </c>
-      <c r="L10" s="4">
+      <c r="O10" s="4">
         <v>120</v>
       </c>
-      <c r="M10" t="b">
-        <v>0</v>
-      </c>
-      <c r="N10" s="3">
-        <v>0</v>
-      </c>
-      <c r="O10">
+      <c r="P10" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>0</v>
+      </c>
+      <c r="R10">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="P10" s="3">
+      <c r="S10" s="3">
         <v>3</v>
       </c>
-      <c r="Q10" s="3">
+      <c r="T10" s="3">
         <v>2000</v>
       </c>
-      <c r="R10" s="3">
+      <c r="U10" s="3">
         <v>1500</v>
       </c>
-      <c r="S10" s="3">
+      <c r="V10" s="3">
         <v>650</v>
       </c>
-      <c r="T10" s="3">
+      <c r="W10" s="3">
         <v>2281</v>
       </c>
-      <c r="U10" s="3">
+      <c r="X10" s="3">
         <v>462</v>
       </c>
-      <c r="V10" s="3">
-        <f t="shared" ref="V10:V13" si="19">3*154</f>
+      <c r="Y10" s="3">
+        <f t="shared" ref="Y10:Y13" si="20">3*154</f>
         <v>462</v>
       </c>
-      <c r="W10" s="3">
-        <v>0</v>
-      </c>
-      <c r="X10" s="4">
+      <c r="Z10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="4">
         <v>2006</v>
       </c>
-      <c r="Y10" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z10" s="1">
+      <c r="AB10" s="11">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AC10" s="1">
+        <f t="shared" si="4"/>
         <v>1819</v>
       </c>
-      <c r="AA10" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AC10" s="3">
-        <f t="shared" ref="AC10:AC13" si="20">345*0.9*2</f>
+      <c r="AD10" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AF10" s="3">
+        <f t="shared" ref="AF10:AF13" si="21">345*0.9*2</f>
         <v>621</v>
       </c>
-      <c r="AD10" s="8">
-        <f t="shared" ref="AD10:AD13" si="21">0.6212*(K10+L10)</f>
+      <c r="AG10" s="8">
+        <f t="shared" ref="AG10:AG13" si="22">0.6212*(N10+O10)</f>
         <v>602.56399999999996</v>
       </c>
-      <c r="AE10" s="8"/>
-      <c r="AF10" s="27">
-        <f t="shared" si="7"/>
+      <c r="AH10" s="8"/>
+      <c r="AI10" s="27">
+        <f t="shared" si="8"/>
         <v>1223.5639999999999</v>
       </c>
-      <c r="AG10" s="15">
-        <f t="shared" si="18"/>
+      <c r="AJ10" s="15">
+        <f t="shared" si="19"/>
         <v>1643.5639999999999</v>
       </c>
-      <c r="AH10" s="4" t="b">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AI10" s="4">
+      <c r="AK10" s="4" t="b">
         <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AL10" s="4">
+        <f t="shared" si="11"/>
         <v>140</v>
       </c>
-      <c r="AJ10" s="8">
+      <c r="AM10" s="8">
         <f t="shared" si="1"/>
         <v>280</v>
       </c>
-      <c r="AK10" s="33">
-        <f t="shared" si="11"/>
+      <c r="AN10" s="33">
+        <f t="shared" si="12"/>
         <v>1819</v>
       </c>
-      <c r="AL10" s="31">
-        <f t="shared" si="12"/>
+      <c r="AO10" s="31">
+        <f t="shared" si="13"/>
         <v>1169</v>
       </c>
-      <c r="AM10" s="33">
-        <f t="shared" si="13"/>
+      <c r="AP10" s="33">
+        <f t="shared" si="14"/>
         <v>1539</v>
       </c>
-      <c r="AN10" s="28">
-        <f t="shared" si="14"/>
+      <c r="AQ10" s="28">
+        <f t="shared" si="15"/>
         <v>889</v>
       </c>
-      <c r="AO10" t="b">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AP10" t="b">
+      <c r="AR10" t="b">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AQ10" t="b">
+      <c r="AS10" t="b">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT10" t="b">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -2006,121 +2114,131 @@
       <c r="J11" s="3">
         <v>12</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M11" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
         <v>850</v>
       </c>
-      <c r="L11" s="4">
+      <c r="O11" s="4">
         <v>120</v>
       </c>
-      <c r="M11" t="b">
-        <v>0</v>
-      </c>
-      <c r="N11" s="3">
-        <v>0</v>
-      </c>
-      <c r="O11">
+      <c r="P11" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>0</v>
+      </c>
+      <c r="R11">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="P11" s="3">
+      <c r="S11" s="3">
         <v>3</v>
       </c>
-      <c r="Q11" s="3">
+      <c r="T11" s="3">
         <v>2000</v>
       </c>
-      <c r="R11" s="3">
+      <c r="U11" s="3">
         <v>1500</v>
       </c>
-      <c r="S11" s="3">
+      <c r="V11" s="3">
         <v>650</v>
       </c>
-      <c r="T11" s="3">
+      <c r="W11" s="3">
         <v>2281</v>
       </c>
-      <c r="U11" s="3">
+      <c r="X11" s="3">
         <v>462</v>
       </c>
-      <c r="V11" s="3">
+      <c r="Y11" s="3">
+        <f t="shared" si="20"/>
+        <v>462</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="4">
+        <v>2006</v>
+      </c>
+      <c r="AB11" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AC11" s="1">
+        <f t="shared" si="4"/>
+        <v>1819</v>
+      </c>
+      <c r="AD11" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AF11" s="3">
+        <f t="shared" si="21"/>
+        <v>621</v>
+      </c>
+      <c r="AG11" s="8">
+        <f t="shared" si="22"/>
+        <v>602.56399999999996</v>
+      </c>
+      <c r="AH11" s="8"/>
+      <c r="AI11" s="27">
+        <f t="shared" si="8"/>
+        <v>1223.5639999999999</v>
+      </c>
+      <c r="AJ11" s="10">
         <f t="shared" si="19"/>
-        <v>462</v>
-      </c>
-      <c r="W11" s="3">
-        <v>0</v>
-      </c>
-      <c r="X11" s="4">
-        <v>2006</v>
-      </c>
-      <c r="Y11" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z11" s="1">
-        <f t="shared" si="3"/>
-        <v>1819</v>
-      </c>
-      <c r="AA11" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AC11" s="3">
-        <f t="shared" si="20"/>
-        <v>621</v>
-      </c>
-      <c r="AD11" s="8">
-        <f t="shared" si="21"/>
-        <v>602.56399999999996</v>
-      </c>
-      <c r="AE11" s="8"/>
-      <c r="AF11" s="27">
-        <f t="shared" si="7"/>
-        <v>1223.5639999999999</v>
-      </c>
-      <c r="AG11" s="10">
-        <f t="shared" si="18"/>
         <v>1643.5639999999999</v>
       </c>
-      <c r="AH11" t="b">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AI11">
+      <c r="AK11" t="b">
         <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AL11">
+        <f t="shared" si="11"/>
         <v>140</v>
       </c>
-      <c r="AJ11" s="8">
+      <c r="AM11" s="8">
         <f t="shared" si="1"/>
         <v>280</v>
       </c>
-      <c r="AK11" s="28">
-        <f t="shared" si="11"/>
+      <c r="AN11" s="28">
+        <f t="shared" si="12"/>
         <v>1819</v>
       </c>
-      <c r="AL11" s="31">
-        <f t="shared" si="12"/>
+      <c r="AO11" s="31">
+        <f t="shared" si="13"/>
         <v>1169</v>
       </c>
-      <c r="AM11" s="28">
-        <f t="shared" si="13"/>
+      <c r="AP11" s="28">
+        <f t="shared" si="14"/>
         <v>1539</v>
       </c>
-      <c r="AN11" s="28">
-        <f t="shared" si="14"/>
+      <c r="AQ11" s="28">
+        <f t="shared" si="15"/>
         <v>889</v>
       </c>
-      <c r="AO11" t="b">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AP11" t="b">
+      <c r="AR11" t="b">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AQ11" t="b">
+      <c r="AS11" t="b">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT11" t="b">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -2151,122 +2269,132 @@
       <c r="J12" s="3">
         <v>10</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
         <v>850</v>
       </c>
-      <c r="L12" s="4">
+      <c r="O12" s="4">
         <v>120</v>
       </c>
-      <c r="M12" t="b">
-        <v>0</v>
-      </c>
-      <c r="N12" s="3">
-        <v>0</v>
-      </c>
-      <c r="O12">
+      <c r="P12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>0</v>
+      </c>
+      <c r="R12">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="P12" s="3">
+      <c r="S12" s="3">
         <v>3</v>
       </c>
-      <c r="Q12" s="3">
+      <c r="T12" s="3">
         <v>2000</v>
       </c>
-      <c r="R12" s="3">
+      <c r="U12" s="3">
         <v>1500</v>
       </c>
-      <c r="S12" s="3">
+      <c r="V12" s="3">
         <v>650</v>
       </c>
-      <c r="T12" s="3">
+      <c r="W12" s="3">
         <v>2281</v>
       </c>
-      <c r="U12" s="3">
+      <c r="X12" s="3">
         <v>462</v>
       </c>
-      <c r="V12" s="3">
+      <c r="Y12" s="3">
+        <f t="shared" si="20"/>
+        <v>462</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="4">
+        <v>2006</v>
+      </c>
+      <c r="AB12" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AC12" s="1">
+        <f t="shared" si="4"/>
+        <v>1819</v>
+      </c>
+      <c r="AD12" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AE12" s="22"/>
+      <c r="AF12" s="3">
+        <f t="shared" si="21"/>
+        <v>621</v>
+      </c>
+      <c r="AG12" s="8">
+        <f t="shared" si="22"/>
+        <v>602.56399999999996</v>
+      </c>
+      <c r="AH12" s="8"/>
+      <c r="AI12" s="27">
+        <f t="shared" si="8"/>
+        <v>1223.5639999999999</v>
+      </c>
+      <c r="AJ12" s="10">
         <f t="shared" si="19"/>
-        <v>462</v>
-      </c>
-      <c r="W12" s="3">
-        <v>0</v>
-      </c>
-      <c r="X12" s="4">
-        <v>2006</v>
-      </c>
-      <c r="Y12" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z12" s="1">
-        <f t="shared" si="3"/>
-        <v>1819</v>
-      </c>
-      <c r="AA12" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB12" s="22"/>
-      <c r="AC12" s="3">
-        <f t="shared" si="20"/>
-        <v>621</v>
-      </c>
-      <c r="AD12" s="8">
-        <f t="shared" si="21"/>
-        <v>602.56399999999996</v>
-      </c>
-      <c r="AE12" s="8"/>
-      <c r="AF12" s="27">
-        <f t="shared" si="7"/>
-        <v>1223.5639999999999</v>
-      </c>
-      <c r="AG12" s="10">
-        <f t="shared" si="18"/>
         <v>1643.5639999999999</v>
       </c>
-      <c r="AH12" t="b">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AI12">
+      <c r="AK12" t="b">
         <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AL12">
+        <f t="shared" si="11"/>
         <v>140</v>
       </c>
-      <c r="AJ12" s="8">
+      <c r="AM12" s="8">
         <f t="shared" si="1"/>
         <v>280</v>
       </c>
-      <c r="AK12" s="28">
-        <f t="shared" si="11"/>
+      <c r="AN12" s="28">
+        <f t="shared" si="12"/>
         <v>1819</v>
       </c>
-      <c r="AL12" s="31">
-        <f t="shared" si="12"/>
+      <c r="AO12" s="31">
+        <f t="shared" si="13"/>
         <v>1169</v>
       </c>
-      <c r="AM12" s="28">
-        <f t="shared" si="13"/>
+      <c r="AP12" s="28">
+        <f t="shared" si="14"/>
         <v>1539</v>
       </c>
-      <c r="AN12" s="28">
-        <f t="shared" si="14"/>
+      <c r="AQ12" s="28">
+        <f t="shared" si="15"/>
         <v>889</v>
       </c>
-      <c r="AO12" t="b">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AP12" t="b">
+      <c r="AR12" t="b">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AQ12" t="b">
+      <c r="AS12" t="b">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT12" t="b">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -2297,122 +2425,132 @@
       <c r="J13" s="3">
         <v>2</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="3">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M13" t="b">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
         <v>850</v>
       </c>
-      <c r="L13" s="4">
+      <c r="O13" s="4">
         <v>120</v>
       </c>
-      <c r="M13" t="b">
-        <v>0</v>
-      </c>
-      <c r="N13" s="3">
-        <v>0</v>
-      </c>
-      <c r="O13">
+      <c r="P13" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>0</v>
+      </c>
+      <c r="R13">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="P13" s="3">
+      <c r="S13" s="3">
         <v>3</v>
       </c>
-      <c r="Q13" s="3">
+      <c r="T13" s="3">
         <v>2000</v>
       </c>
-      <c r="R13" s="3">
+      <c r="U13" s="3">
         <v>1500</v>
       </c>
-      <c r="S13" s="3">
+      <c r="V13" s="3">
         <v>650</v>
       </c>
-      <c r="T13" s="3">
+      <c r="W13" s="3">
         <v>2281</v>
       </c>
-      <c r="U13" s="3">
+      <c r="X13" s="3">
         <v>462</v>
       </c>
-      <c r="V13" s="3">
+      <c r="Y13" s="3">
+        <f t="shared" si="20"/>
+        <v>462</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="4">
+        <v>2006</v>
+      </c>
+      <c r="AB13" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AC13" s="1">
+        <f t="shared" si="4"/>
+        <v>1819</v>
+      </c>
+      <c r="AD13" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AE13" s="22"/>
+      <c r="AF13" s="3">
+        <f t="shared" si="21"/>
+        <v>621</v>
+      </c>
+      <c r="AG13" s="8">
+        <f t="shared" si="22"/>
+        <v>602.56399999999996</v>
+      </c>
+      <c r="AH13" s="8"/>
+      <c r="AI13" s="27">
+        <f t="shared" si="8"/>
+        <v>1223.5639999999999</v>
+      </c>
+      <c r="AJ13" s="10">
         <f t="shared" si="19"/>
-        <v>462</v>
-      </c>
-      <c r="W13" s="3">
-        <v>0</v>
-      </c>
-      <c r="X13" s="4">
-        <v>2006</v>
-      </c>
-      <c r="Y13" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z13" s="1">
-        <f t="shared" si="3"/>
-        <v>1819</v>
-      </c>
-      <c r="AA13" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB13" s="22"/>
-      <c r="AC13" s="3">
-        <f t="shared" si="20"/>
-        <v>621</v>
-      </c>
-      <c r="AD13" s="8">
-        <f t="shared" si="21"/>
-        <v>602.56399999999996</v>
-      </c>
-      <c r="AE13" s="8"/>
-      <c r="AF13" s="27">
-        <f t="shared" si="7"/>
-        <v>1223.5639999999999</v>
-      </c>
-      <c r="AG13" s="10">
-        <f t="shared" si="18"/>
         <v>1643.5639999999999</v>
       </c>
-      <c r="AH13" t="b">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AI13">
+      <c r="AK13" t="b">
         <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AL13">
+        <f t="shared" si="11"/>
         <v>140</v>
       </c>
-      <c r="AJ13" s="8">
+      <c r="AM13" s="8">
         <f t="shared" si="1"/>
         <v>280</v>
       </c>
-      <c r="AK13" s="28">
-        <f t="shared" si="11"/>
+      <c r="AN13" s="28">
+        <f t="shared" si="12"/>
         <v>1819</v>
       </c>
-      <c r="AL13" s="31">
-        <f t="shared" si="12"/>
+      <c r="AO13" s="31">
+        <f t="shared" si="13"/>
         <v>1169</v>
       </c>
-      <c r="AM13" s="28">
-        <f t="shared" si="13"/>
+      <c r="AP13" s="28">
+        <f t="shared" si="14"/>
         <v>1539</v>
       </c>
-      <c r="AN13" s="28">
-        <f t="shared" si="14"/>
+      <c r="AQ13" s="28">
+        <f t="shared" si="15"/>
         <v>889</v>
       </c>
-      <c r="AO13" t="b">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AP13" t="b">
+      <c r="AR13" t="b">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AQ13" t="b">
+      <c r="AS13" t="b">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT13" t="b">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>5</v>
       </c>
@@ -2444,109 +2582,119 @@
         <v>30</v>
       </c>
       <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="2"/>
+        <v>2000</v>
+      </c>
+      <c r="M14" t="b">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2">
         <v>720</v>
       </c>
-      <c r="L14" s="2">
+      <c r="O14" s="2">
         <v>110</v>
       </c>
-      <c r="M14" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N14" s="2">
-        <v>0</v>
-      </c>
-      <c r="O14" s="2">
+      <c r="P14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>0</v>
+      </c>
+      <c r="R14" s="2">
         <v>3</v>
       </c>
-      <c r="P14" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="2">
+      <c r="S14" s="2">
+        <v>0</v>
+      </c>
+      <c r="T14" s="2">
         <v>2500</v>
-      </c>
-      <c r="R14" s="2">
-        <v>1578</v>
-      </c>
-      <c r="S14" s="2">
-        <v>400</v>
-      </c>
-      <c r="T14" s="2">
-        <v>1703</v>
       </c>
       <c r="U14" s="2">
         <v>1578</v>
       </c>
       <c r="V14" s="2">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="W14" s="2">
-        <v>0</v>
+        <v>1703</v>
       </c>
       <c r="X14" s="2">
+        <v>1578</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="2">
         <v>2011</v>
       </c>
-      <c r="Y14" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z14" s="1">
+      <c r="AB14" s="18">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AA14" s="18">
+      <c r="AC14" s="1">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AD14" s="18">
+        <f t="shared" si="5"/>
         <v>400</v>
       </c>
-      <c r="AB14" s="7"/>
-      <c r="AC14" s="7">
+      <c r="AE14" s="7"/>
+      <c r="AF14" s="7">
         <f>3*291</f>
         <v>873</v>
       </c>
-      <c r="AD14" s="2"/>
-      <c r="AE14" s="2"/>
-      <c r="AF14" s="25">
-        <f t="shared" si="7"/>
-        <v>873</v>
-      </c>
       <c r="AG14" s="2"/>
       <c r="AH14" s="2"/>
-      <c r="AI14" s="4">
-        <f t="shared" si="10"/>
+      <c r="AI14" s="25">
+        <f t="shared" si="8"/>
+        <v>873</v>
+      </c>
+      <c r="AJ14" s="2"/>
+      <c r="AK14" s="2"/>
+      <c r="AL14" s="4">
+        <f t="shared" si="11"/>
         <v>355</v>
       </c>
-      <c r="AJ14" s="8">
-        <v>0</v>
-      </c>
-      <c r="AK14" s="28">
-        <f t="shared" si="11"/>
+      <c r="AM14" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN14" s="28">
+        <f t="shared" si="12"/>
         <v>125</v>
       </c>
-      <c r="AL14" s="28">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AM14" s="28">
+      <c r="AO14" s="28">
         <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AP14" s="28">
+        <f t="shared" si="14"/>
         <v>125</v>
       </c>
-      <c r="AN14" s="28">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AO14" t="b">
+      <c r="AQ14" s="28">
         <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="AP14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR14" t="b">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AQ14" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS14" t="b">
         <f t="shared" si="17"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="AT14" t="b">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>5</v>
       </c>
@@ -2577,106 +2725,116 @@
       <c r="J15" s="3">
         <v>40</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="3">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>2000</v>
+      </c>
+      <c r="M15" t="b">
+        <v>0</v>
+      </c>
+      <c r="N15">
         <v>720</v>
       </c>
-      <c r="L15">
+      <c r="O15">
         <v>110</v>
       </c>
-      <c r="M15" t="b">
-        <v>0</v>
-      </c>
-      <c r="N15" s="3">
-        <v>0</v>
-      </c>
-      <c r="O15">
+      <c r="P15" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>0</v>
+      </c>
+      <c r="R15">
         <v>3</v>
       </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="3">
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15" s="3">
         <v>2500</v>
-      </c>
-      <c r="R15" s="3">
-        <v>1578</v>
-      </c>
-      <c r="S15" s="3">
-        <v>400</v>
-      </c>
-      <c r="T15">
-        <v>1703</v>
       </c>
       <c r="U15" s="3">
         <v>1578</v>
       </c>
-      <c r="V15">
-        <v>0</v>
-      </c>
-      <c r="W15" s="3">
-        <v>0</v>
-      </c>
-      <c r="X15" s="2">
+      <c r="V15" s="3">
+        <v>400</v>
+      </c>
+      <c r="W15">
+        <v>1703</v>
+      </c>
+      <c r="X15" s="3">
+        <v>1578</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="2">
         <v>2011</v>
       </c>
-      <c r="Y15" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z15" s="1">
+      <c r="AB15" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AA15" s="1">
+      <c r="AC15" s="1">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AD15" s="1">
+        <f t="shared" si="5"/>
         <v>400</v>
       </c>
-      <c r="AB15" s="3"/>
-      <c r="AC15">
-        <f t="shared" ref="AC15:AC16" si="22">3*291</f>
+      <c r="AE15" s="3"/>
+      <c r="AF15">
+        <f t="shared" ref="AF15:AF16" si="23">3*291</f>
         <v>873</v>
       </c>
-      <c r="AF15" s="24">
-        <f t="shared" si="7"/>
+      <c r="AI15" s="24">
+        <f t="shared" si="8"/>
         <v>873</v>
       </c>
-      <c r="AI15">
-        <f t="shared" si="10"/>
+      <c r="AL15">
+        <f t="shared" si="11"/>
         <v>355</v>
       </c>
-      <c r="AJ15" s="8">
-        <v>0</v>
-      </c>
-      <c r="AK15" s="28">
-        <f t="shared" si="11"/>
+      <c r="AM15" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN15" s="28">
+        <f t="shared" si="12"/>
         <v>125</v>
       </c>
-      <c r="AL15" s="28">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AM15" s="28">
+      <c r="AO15" s="28">
         <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AP15" s="28">
+        <f t="shared" si="14"/>
         <v>125</v>
       </c>
-      <c r="AN15" s="28">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AO15" t="b">
+      <c r="AQ15" s="28">
         <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="AP15" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR15" t="b">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AQ15" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS15" t="b">
         <f t="shared" si="17"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="AT15" t="b">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>5</v>
       </c>
@@ -2707,106 +2865,116 @@
       <c r="J16" s="3">
         <v>35</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="3">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="2"/>
+        <v>2000</v>
+      </c>
+      <c r="M16" t="b">
+        <v>0</v>
+      </c>
+      <c r="N16">
         <v>720</v>
       </c>
-      <c r="L16">
+      <c r="O16">
         <v>110</v>
       </c>
-      <c r="M16" t="b">
-        <v>0</v>
-      </c>
-      <c r="N16" s="3">
-        <v>0</v>
-      </c>
-      <c r="O16">
+      <c r="P16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>0</v>
+      </c>
+      <c r="R16">
         <v>3</v>
       </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="3">
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16" s="3">
         <v>2500</v>
-      </c>
-      <c r="R16" s="3">
-        <v>1578</v>
-      </c>
-      <c r="S16" s="3">
-        <v>400</v>
-      </c>
-      <c r="T16">
-        <v>1703</v>
       </c>
       <c r="U16" s="3">
         <v>1578</v>
       </c>
-      <c r="V16">
-        <v>0</v>
-      </c>
-      <c r="W16" s="3">
-        <v>0</v>
-      </c>
-      <c r="X16" s="2">
+      <c r="V16" s="3">
+        <v>400</v>
+      </c>
+      <c r="W16">
+        <v>1703</v>
+      </c>
+      <c r="X16" s="3">
+        <v>1578</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="2">
         <v>2011</v>
       </c>
-      <c r="Y16" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z16" s="1">
+      <c r="AB16" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AA16" s="1">
+      <c r="AC16" s="1">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AD16" s="1">
+        <f t="shared" si="5"/>
         <v>400</v>
       </c>
-      <c r="AB16" s="3"/>
-      <c r="AC16">
-        <f t="shared" si="22"/>
+      <c r="AE16" s="3"/>
+      <c r="AF16">
+        <f t="shared" si="23"/>
         <v>873</v>
       </c>
-      <c r="AF16" s="24">
-        <f t="shared" si="7"/>
+      <c r="AI16" s="24">
+        <f t="shared" si="8"/>
         <v>873</v>
       </c>
-      <c r="AI16">
-        <f t="shared" si="10"/>
+      <c r="AL16">
+        <f t="shared" si="11"/>
         <v>355</v>
       </c>
-      <c r="AJ16" s="8">
-        <v>0</v>
-      </c>
-      <c r="AK16" s="28">
-        <f t="shared" si="11"/>
+      <c r="AM16" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN16" s="28">
+        <f t="shared" si="12"/>
         <v>125</v>
       </c>
-      <c r="AL16" s="28">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AM16" s="28">
+      <c r="AO16" s="28">
         <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AP16" s="28">
+        <f t="shared" si="14"/>
         <v>125</v>
       </c>
-      <c r="AN16" s="28">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AO16" t="b">
+      <c r="AQ16" s="28">
         <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="AP16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR16" t="b">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AQ16" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS16" t="b">
         <f t="shared" si="17"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="AT16" t="b">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>6</v>
       </c>
@@ -2838,119 +3006,129 @@
         <v>28</v>
       </c>
       <c r="K17" s="2">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="2"/>
+        <v>2000</v>
+      </c>
+      <c r="M17" t="b">
+        <v>0</v>
+      </c>
+      <c r="N17" s="2">
         <v>400</v>
       </c>
-      <c r="L17" s="2">
+      <c r="O17" s="2">
         <v>80</v>
       </c>
-      <c r="M17" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="N17" s="2">
+      <c r="P17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="2">
         <v>0.36</v>
       </c>
-      <c r="O17" s="2">
-        <f t="shared" ref="O17:O18" si="23">G17-P17</f>
-        <v>1</v>
-      </c>
-      <c r="P17" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="2">
+      <c r="R17" s="2">
+        <f t="shared" ref="R17:R18" si="24">G17-S17</f>
+        <v>1</v>
+      </c>
+      <c r="S17" s="2">
+        <v>1</v>
+      </c>
+      <c r="T17" s="2">
         <v>1000</v>
       </c>
-      <c r="R17" s="2">
+      <c r="U17" s="2">
         <v>719</v>
       </c>
-      <c r="S17" s="2">
+      <c r="V17" s="2">
         <f>500-(0.9*160)</f>
         <v>356</v>
       </c>
-      <c r="T17" s="2">
+      <c r="W17" s="2">
         <v>1183.6399999999999</v>
       </c>
-      <c r="U17" s="2">
+      <c r="X17" s="2">
         <v>555</v>
       </c>
-      <c r="V17" s="2">
+      <c r="Y17" s="2">
         <v>194</v>
       </c>
-      <c r="W17" s="2">
-        <v>0</v>
-      </c>
-      <c r="X17" s="2">
+      <c r="Z17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="2">
         <v>2019</v>
       </c>
-      <c r="Y17" s="20">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="1">
-        <f t="shared" si="3"/>
+      <c r="AB17" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="1">
+        <f t="shared" si="4"/>
         <v>628.63999999999987</v>
       </c>
-      <c r="AA17" s="18">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB17" s="2"/>
-      <c r="AC17" s="4">
-        <f>359*(1+N17)</f>
+      <c r="AD17" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AE17" s="2"/>
+      <c r="AF17" s="4">
+        <f>359*(1+Q17)</f>
         <v>488.23999999999995</v>
       </c>
-      <c r="AD17" s="9">
-        <f>0.759*(K17+L17)</f>
+      <c r="AG17" s="9">
+        <f>0.759*(N17+O17)</f>
         <v>364.32</v>
       </c>
-      <c r="AE17" s="8"/>
-      <c r="AF17" s="25">
-        <f t="shared" ref="AF17:AF18" si="24">AC17+AD17</f>
+      <c r="AH17" s="8"/>
+      <c r="AI17" s="25">
+        <f t="shared" ref="AI17:AI18" si="25">AF17+AG17</f>
         <v>852.56</v>
       </c>
-      <c r="AG17" s="10">
-        <f>AF17+140*P17</f>
+      <c r="AJ17" s="10">
+        <f>AI17+140*S17</f>
         <v>992.56</v>
       </c>
-      <c r="AH17" t="b">
-        <f>AND((Q17&gt;600),(R17&lt;=AG17))</f>
-        <v>1</v>
-      </c>
-      <c r="AI17">
-        <f t="shared" ref="AI17" si="25">ROUND(MAX(R17-AF17,0)/10,0)*5</f>
-        <v>0</v>
-      </c>
-      <c r="AJ17" s="9">
-        <v>0</v>
-      </c>
-      <c r="AK17" s="29">
-        <f t="shared" ref="AK17:AK18" si="26">MAX(T17-U17,0)</f>
+      <c r="AK17" t="b">
+        <f>AND((T17&gt;600),(U17&lt;=AJ17))</f>
+        <v>1</v>
+      </c>
+      <c r="AL17">
+        <f t="shared" ref="AL17" si="26">ROUND(MAX(U17-AI17,0)/10,0)*5</f>
+        <v>0</v>
+      </c>
+      <c r="AM17" s="9">
+        <v>0</v>
+      </c>
+      <c r="AN17" s="29">
+        <f t="shared" ref="AN17:AN18" si="27">MAX(W17-X17,0)</f>
         <v>628.63999999999987</v>
       </c>
-      <c r="AL17" s="29">
-        <f t="shared" ref="AL17:AL18" si="27">MAX(T17-U17-S17,0)</f>
+      <c r="AO17" s="29">
+        <f t="shared" ref="AO17:AO18" si="28">MAX(W17-X17-V17,0)</f>
         <v>272.63999999999987</v>
       </c>
-      <c r="AM17" s="29">
-        <f t="shared" ref="AM17:AM18" si="28">MAX(T17-U17-AJ17,0)</f>
+      <c r="AP17" s="29">
+        <f t="shared" ref="AP17:AP18" si="29">MAX(W17-X17-AM17,0)</f>
         <v>628.63999999999987</v>
       </c>
-      <c r="AN17" s="28">
-        <f t="shared" ref="AN17:AN18" si="29">MAX(T17-U17-S17-AJ17,0)</f>
+      <c r="AQ17" s="28">
+        <f t="shared" ref="AQ17:AQ18" si="30">MAX(W17-X17-V17-AM17,0)</f>
         <v>272.63999999999987</v>
       </c>
-      <c r="AO17" t="b">
-        <f t="shared" ref="AO17:AO18" si="30">AND(AL17=0,AK17&gt;0)</f>
-        <v>0</v>
-      </c>
-      <c r="AP17" t="b">
-        <f t="shared" ref="AP17:AP18" si="31">AND(AM17=0,AK17&gt;0)</f>
-        <v>0</v>
-      </c>
-      <c r="AQ17" t="b">
-        <f t="shared" ref="AQ17:AQ18" si="32">AND(AN17=0,AK17&gt;0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR17" t="b">
+        <f t="shared" ref="AR17:AR18" si="31">AND(AO17=0,AN17&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="AS17" t="b">
+        <f t="shared" ref="AS17:AS18" si="32">AND(AP17=0,AN17&gt;0)</f>
+        <v>0</v>
+      </c>
+      <c r="AT17" t="b">
+        <f t="shared" ref="AT17:AT18" si="33">AND(AQ17=0,AN17&gt;0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
@@ -2982,218 +3160,228 @@
         <v>1</v>
       </c>
       <c r="K18" s="3">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M18" t="b">
+        <v>0</v>
+      </c>
+      <c r="N18" s="3">
         <v>400</v>
       </c>
-      <c r="L18" s="3">
+      <c r="O18" s="3">
         <v>80</v>
       </c>
-      <c r="M18" t="b">
-        <v>1</v>
-      </c>
-      <c r="N18" s="3">
+      <c r="P18" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="3">
         <v>0.36</v>
       </c>
-      <c r="O18">
-        <f t="shared" si="23"/>
-        <v>1</v>
-      </c>
-      <c r="P18" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="3">
+      <c r="R18">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="S18" s="3">
+        <v>1</v>
+      </c>
+      <c r="T18" s="3">
         <v>1000</v>
       </c>
-      <c r="R18" s="3">
+      <c r="U18" s="3">
         <v>719</v>
       </c>
-      <c r="S18" s="3">
+      <c r="V18" s="3">
         <v>256</v>
       </c>
-      <c r="T18" s="3">
+      <c r="W18" s="3">
         <v>1183.6399999999999</v>
       </c>
-      <c r="U18" s="2">
+      <c r="X18" s="2">
         <v>555</v>
       </c>
-      <c r="V18" s="3">
+      <c r="Y18" s="3">
         <v>194</v>
       </c>
-      <c r="W18" s="3">
+      <c r="Z18" s="3">
         <v>160</v>
       </c>
-      <c r="X18" s="3">
+      <c r="AA18" s="3">
         <v>2019</v>
       </c>
-      <c r="Y18" s="21">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="1">
-        <f t="shared" si="3"/>
+      <c r="AB18" s="21">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="1">
+        <f t="shared" si="4"/>
         <v>628.63999999999987</v>
       </c>
-      <c r="AA18" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AC18" s="4">
-        <f>359*(1+N18)</f>
+      <c r="AD18" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AF18" s="4">
+        <f>359*(1+Q18)</f>
         <v>488.23999999999995</v>
       </c>
-      <c r="AD18" s="8">
-        <f>0.759*(K18+L18)</f>
+      <c r="AG18" s="8">
+        <f>0.759*(N18+O18)</f>
         <v>364.32</v>
       </c>
-      <c r="AE18" s="8"/>
-      <c r="AF18" s="27">
-        <f t="shared" si="24"/>
+      <c r="AH18" s="8"/>
+      <c r="AI18" s="27">
+        <f t="shared" si="25"/>
         <v>852.56</v>
       </c>
-      <c r="AG18" s="10">
-        <f>AF18+140*P18</f>
+      <c r="AJ18" s="10">
+        <f>AI18+140*S18</f>
         <v>992.56</v>
       </c>
-      <c r="AH18" s="3" t="b">
-        <f>AND((Q18&gt;600),(R18&lt;=AG18))</f>
-        <v>1</v>
-      </c>
-      <c r="AI18" s="3">
-        <f>ROUND(MAX(R18-AF18,0)/10,0)*5</f>
-        <v>0</v>
-      </c>
-      <c r="AJ18" s="8">
-        <v>0</v>
-      </c>
-      <c r="AK18" s="31">
-        <f t="shared" si="26"/>
+      <c r="AK18" s="3" t="b">
+        <f>AND((T18&gt;600),(U18&lt;=AJ18))</f>
+        <v>1</v>
+      </c>
+      <c r="AL18" s="3">
+        <f>ROUND(MAX(U18-AI18,0)/10,0)*5</f>
+        <v>0</v>
+      </c>
+      <c r="AM18" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN18" s="31">
+        <f t="shared" si="27"/>
         <v>628.63999999999987</v>
       </c>
-      <c r="AL18" s="31">
-        <f t="shared" si="27"/>
+      <c r="AO18" s="31">
+        <f t="shared" si="28"/>
         <v>372.63999999999987</v>
       </c>
-      <c r="AM18" s="31">
-        <f t="shared" si="28"/>
+      <c r="AP18" s="31">
+        <f t="shared" si="29"/>
         <v>628.63999999999987</v>
       </c>
-      <c r="AN18" s="28">
-        <f t="shared" si="29"/>
+      <c r="AQ18" s="28">
+        <f t="shared" si="30"/>
         <v>372.63999999999987</v>
       </c>
-      <c r="AO18" t="b">
-        <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="AP18" t="b">
+      <c r="AR18" t="b">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="AQ18" t="b">
+      <c r="AS18" t="b">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AB19" s="22"/>
-      <c r="AF19" s="24"/>
-      <c r="AJ19" s="8"/>
-    </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AB20" s="22"/>
-      <c r="AF20" s="8"/>
-      <c r="AJ20" s="8"/>
-    </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AB21" s="22"/>
-      <c r="AF21" s="8"/>
-      <c r="AJ21" s="8"/>
-    </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AF22" s="8"/>
-      <c r="AJ22" s="8"/>
-    </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AF23" s="8"/>
-      <c r="AJ23" s="8"/>
-    </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AF24" s="8"/>
-      <c r="AJ24" s="8"/>
-    </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AF25" s="8"/>
+      <c r="AT18" t="b">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AE19" s="22"/>
+      <c r="AI19" s="24"/>
+      <c r="AM19" s="8"/>
+    </row>
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AE20" s="22"/>
+      <c r="AI20" s="8"/>
+      <c r="AM20" s="8"/>
+    </row>
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AE21" s="22"/>
+      <c r="AI21" s="8"/>
+      <c r="AM21" s="8"/>
+    </row>
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AI22" s="8"/>
+      <c r="AM22" s="8"/>
+    </row>
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AI23" s="8"/>
+      <c r="AM23" s="8"/>
+    </row>
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AI24" s="8"/>
+      <c r="AM24" s="8"/>
+    </row>
+    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
       <c r="AI25" s="8"/>
-      <c r="AJ25" s="8"/>
-    </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AF26" s="8"/>
+      <c r="AL25" s="8"/>
+      <c r="AM25" s="8"/>
+    </row>
+    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
       <c r="AI26" s="8"/>
-      <c r="AJ26" s="8"/>
-    </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AF27" s="8"/>
+      <c r="AL26" s="8"/>
+      <c r="AM26" s="8"/>
+    </row>
+    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
       <c r="AI27" s="8"/>
-      <c r="AJ27" s="8"/>
-    </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AF28" s="8"/>
+      <c r="AL27" s="8"/>
+      <c r="AM27" s="8"/>
+    </row>
+    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
       <c r="AI28" s="8"/>
-      <c r="AJ28" s="8"/>
-    </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AF29" s="8"/>
+      <c r="AL28" s="8"/>
+      <c r="AM28" s="8"/>
+    </row>
+    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
       <c r="AI29" s="8"/>
-    </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AF30" s="8"/>
+      <c r="AL29" s="8"/>
+    </row>
+    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
       <c r="AI30" s="8"/>
-    </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AF31" s="8"/>
+      <c r="AL30" s="8"/>
+    </row>
+    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
       <c r="AI31" s="8"/>
-    </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AF32" s="8"/>
+      <c r="AL31" s="8"/>
+    </row>
+    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
       <c r="AI32" s="8"/>
-    </row>
-    <row r="33" spans="32:35" x14ac:dyDescent="0.25">
-      <c r="AF33" s="8"/>
+      <c r="AL32" s="8"/>
+    </row>
+    <row r="33" spans="35:38" x14ac:dyDescent="0.25">
       <c r="AI33" s="8"/>
-    </row>
-    <row r="34" spans="32:35" x14ac:dyDescent="0.25">
-      <c r="AF34" s="8"/>
+      <c r="AL33" s="8"/>
+    </row>
+    <row r="34" spans="35:38" x14ac:dyDescent="0.25">
       <c r="AI34" s="8"/>
-    </row>
-    <row r="35" spans="32:35" x14ac:dyDescent="0.25">
-      <c r="AF35" s="8"/>
+      <c r="AL34" s="8"/>
+    </row>
+    <row r="35" spans="35:38" x14ac:dyDescent="0.25">
       <c r="AI35" s="8"/>
-    </row>
-    <row r="36" spans="32:35" x14ac:dyDescent="0.25">
-      <c r="AF36" s="8"/>
+      <c r="AL35" s="8"/>
+    </row>
+    <row r="36" spans="35:38" x14ac:dyDescent="0.25">
       <c r="AI36" s="8"/>
-    </row>
-    <row r="37" spans="32:35" x14ac:dyDescent="0.25">
-      <c r="AF37" s="8"/>
+      <c r="AL36" s="8"/>
+    </row>
+    <row r="37" spans="35:38" x14ac:dyDescent="0.25">
       <c r="AI37" s="8"/>
-    </row>
-    <row r="38" spans="32:35" x14ac:dyDescent="0.25">
-      <c r="AF38" s="8"/>
+      <c r="AL37" s="8"/>
+    </row>
+    <row r="38" spans="35:38" x14ac:dyDescent="0.25">
       <c r="AI38" s="8"/>
-    </row>
-    <row r="39" spans="32:35" x14ac:dyDescent="0.25">
-      <c r="AF39" s="8"/>
+      <c r="AL38" s="8"/>
+    </row>
+    <row r="39" spans="35:38" x14ac:dyDescent="0.25">
       <c r="AI39" s="8"/>
-    </row>
-    <row r="40" spans="32:35" x14ac:dyDescent="0.25">
-      <c r="AF40" s="8"/>
+      <c r="AL39" s="8"/>
+    </row>
+    <row r="40" spans="35:38" x14ac:dyDescent="0.25">
       <c r="AI40" s="8"/>
-    </row>
-    <row r="41" spans="32:35" x14ac:dyDescent="0.25">
-      <c r="AF41" s="8"/>
+      <c r="AL40" s="8"/>
+    </row>
+    <row r="41" spans="35:38" x14ac:dyDescent="0.25">
       <c r="AI41" s="8"/>
-    </row>
-    <row r="42" spans="32:35" x14ac:dyDescent="0.25">
-      <c r="AF42" s="8"/>
+      <c r="AL41" s="8"/>
+    </row>
+    <row r="42" spans="35:38" x14ac:dyDescent="0.25">
       <c r="AI42" s="8"/>
+      <c r="AL42" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>